<commit_message>
Adds more tests for database
</commit_message>
<xml_diff>
--- a/LINQ_TO_SQL/AverageScoreBySpecialty.xlsx
+++ b/LINQ_TO_SQL/AverageScoreBySpecialty.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Year</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>IP-21</t>
-  </si>
-  <si>
-    <t>IP-31</t>
   </si>
   <si>
     <t>Winter/2020</t>
@@ -81,7 +78,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -103,7 +100,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="0">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>4</v>
@@ -111,35 +108,13 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="0">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="0">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>